<commit_message>
admin user ngga bisa import
</commit_message>
<xml_diff>
--- a/file/format_user_data.xlsx
+++ b/file/format_user_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pengaduan\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB76D35F-BABA-4C64-88ED-1CA6AD72A829}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4066865-139D-4B35-BD12-6D542D3DAC87}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{527C6868-5F6A-45DD-BB60-3EC0BD397F85}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>id_user</t>
   </si>
@@ -36,40 +36,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>id_level</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>token</t>
-  </si>
-  <si>
     <t>[boleh kosong]</t>
   </si>
   <si>
-    <t>NIP/NIM 6 digit</t>
-  </si>
-  <si>
-    <t>keterangan:</t>
-  </si>
-  <si>
-    <t>aktif</t>
-  </si>
-  <si>
-    <t>status = 1 =</t>
-  </si>
-  <si>
-    <t>level</t>
+    <t>id_role</t>
   </si>
 </sst>
 </file>
@@ -441,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFB583-5C7D-436C-AFA6-EECB7079903A}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +435,7 @@
     <col min="11" max="11" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -467,60 +443,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1"/>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
import done, cek bug list lagi
</commit_message>
<xml_diff>
--- a/file/format_user_data.xlsx
+++ b/file/format_user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pengaduan\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4066865-139D-4B35-BD12-6D542D3DAC87}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE96C1B5-4A20-4315-95FA-9852086C6EF2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{527C6868-5F6A-45DD-BB60-3EC0BD397F85}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>id_user</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nama_pengguna</t>
   </si>
@@ -40,9 +37,6 @@
   </si>
   <si>
     <t>username</t>
-  </si>
-  <si>
-    <t>[boleh kosong]</t>
   </si>
   <si>
     <t>id_role</t>
@@ -417,52 +411,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFB583-5C7D-436C-AFA6-EECB7079903A}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>